<commit_message>
fix variable for client/patient:clinic demographic update
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/clinic-edit.xlsx
+++ b/config/default/forms/contact/clinic-edit.xlsx
@@ -138,24 +138,27 @@
     <t xml:space="preserve">Demographics update</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_demographics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**&lt;span style="color:blue"&gt;Demographics&lt;/span&gt;**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patient_familyName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surname</t>
+  </si>
+  <si>
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n_demographics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**&lt;span style="color:blue"&gt;Demographics&lt;/span&gt;**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient_familyName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surname</t>
-  </si>
-  <si>
     <t xml:space="preserve">regex(., ‘^[A-Z]{1}[a-z]{1,14}$’)</t>
   </si>
   <si>
@@ -196,9 +199,6 @@
   </si>
   <si>
     <t xml:space="preserve">National ID No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">regex(.,'^[0-9]{5,10}$')</t>
@@ -4952,20 +4952,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="79.8265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.3061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="52.3775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="119.423469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.7704081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.3163265306123"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.7704081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="47.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="22.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.984693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="82.7040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.3877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="123.739795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="41.6683673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="49.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="23.4897959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5362,15 +5362,15 @@
         <v>43</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -5384,21 +5384,21 @@
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -5412,19 +5412,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -5435,7 +5435,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>1</v>
@@ -5449,7 +5449,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -5459,10 +5459,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>16</v>
@@ -5473,7 +5473,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -5486,10 +5486,10 @@
         <v>39</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -5508,13 +5508,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -5542,7 +5542,7 @@
         <v>62</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -5591,7 +5591,7 @@
         <v>69</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -5615,7 +5615,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -5639,7 +5639,7 @@
         <v>75</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>76</v>
@@ -5669,7 +5669,7 @@
         <v>81</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>82</v>
@@ -5699,7 +5699,7 @@
         <v>86</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>82</v>
@@ -5720,7 +5720,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>89</v>
@@ -5744,7 +5744,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>91</v>
@@ -5768,7 +5768,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>93</v>
@@ -5792,7 +5792,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>96</v>
@@ -5816,7 +5816,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>98</v>
@@ -5865,7 +5865,7 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>102</v>
@@ -5889,7 +5889,7 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>105</v>
@@ -5913,7 +5913,7 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>108</v>
@@ -6112,7 +6112,7 @@
         <v>132</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -6142,7 +6142,7 @@
         <v>136</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -6172,7 +6172,7 @@
         <v>139</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -6196,7 +6196,7 @@
         <v>141</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -6220,7 +6220,7 @@
         <v>144</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3" t="s">
@@ -6246,7 +6246,7 @@
         <v>147</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3" t="s">
@@ -6274,7 +6274,7 @@
         <v>150</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -6298,7 +6298,7 @@
         <v>152</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -6322,7 +6322,7 @@
         <v>154</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -6346,7 +6346,7 @@
         <v>156</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -6370,7 +6370,7 @@
         <v>158</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -6394,7 +6394,7 @@
         <v>160</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -6442,7 +6442,7 @@
         <v>165</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -6526,7 +6526,7 @@
         <v>170</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -6554,7 +6554,7 @@
         <v>175</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>176</v>
@@ -6582,7 +6582,7 @@
         <v>175</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>179</v>
@@ -6601,7 +6601,7 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>180</v>
@@ -6715,7 +6715,7 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>187</v>
@@ -6739,7 +6739,7 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>189</v>
@@ -6763,7 +6763,7 @@
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>191</v>
@@ -6883,7 +6883,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
-      <formula>AND($A45="end repeat", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
+      <formula>and($A45="end repeat", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
@@ -7805,10 +7805,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.5867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.9489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.9081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="22.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.1581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="23.4897959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28478,9 +28478,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.6275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="22.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.8877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="23.4897959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28515,7 +28515,7 @@
       </c>
       <c r="C2" s="32" t="n">
         <f aca="true">NOW()</f>
-        <v>44098.66703421</v>
+        <v>44098.7187694888</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>833</v>

</xml_diff>

<commit_message>
fix for demographics update variable
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/clinic-edit.xlsx
+++ b/config/default/forms/contact/clinic-edit.xlsx
@@ -132,6 +132,9 @@
     <t xml:space="preserve">cht</t>
   </si>
   <si>
+    <t xml:space="preserve">calculate</t>
+  </si>
+  <si>
     <t xml:space="preserve">new_registration</t>
   </si>
   <si>
@@ -175,9 +178,6 @@
   </si>
   <si>
     <t xml:space="preserve">Other name(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculate</t>
   </si>
   <si>
     <t xml:space="preserve">concat(${patient_familyName}, ' ', ${patient_middleName}, ' ', ${patient_firstName})</t>
@@ -4947,25 +4947,25 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.984693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="82.7040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.3877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="123.739795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="41.6683673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="49.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.6734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.3367346938775"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.2448979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="128.15306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="43.1071428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="24.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5307,37 +5307,37 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="11"/>
+      <c r="I15" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="J15" s="8"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="L15" s="12"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="3"/>
@@ -5356,21 +5356,21 @@
         <v>18</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -5384,21 +5384,21 @@
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -5412,19 +5412,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -5435,7 +5435,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>1</v>
@@ -5459,7 +5459,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>53</v>
@@ -5483,7 +5483,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>55</v>
@@ -5514,7 +5514,7 @@
         <v>58</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -5542,7 +5542,7 @@
         <v>62</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -5560,7 +5560,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>65</v>
@@ -5591,7 +5591,7 @@
         <v>69</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -5615,7 +5615,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -5639,7 +5639,7 @@
         <v>75</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>76</v>
@@ -5669,7 +5669,7 @@
         <v>81</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>82</v>
@@ -5699,7 +5699,7 @@
         <v>86</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>82</v>
@@ -5720,7 +5720,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>89</v>
@@ -5744,7 +5744,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>91</v>
@@ -5768,7 +5768,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>93</v>
@@ -5792,7 +5792,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>96</v>
@@ -5816,7 +5816,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>98</v>
@@ -5840,7 +5840,7 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>100</v>
@@ -5865,7 +5865,7 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>102</v>
@@ -5889,7 +5889,7 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>105</v>
@@ -5913,7 +5913,7 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>108</v>
@@ -6035,7 +6035,7 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>124</v>
@@ -6057,7 +6057,7 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>125</v>
@@ -6112,7 +6112,7 @@
         <v>132</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -6142,7 +6142,7 @@
         <v>136</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -6172,7 +6172,7 @@
         <v>139</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -6196,7 +6196,7 @@
         <v>141</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -6220,7 +6220,7 @@
         <v>144</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3" t="s">
@@ -6246,7 +6246,7 @@
         <v>147</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3" t="s">
@@ -6274,7 +6274,7 @@
         <v>150</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -6298,7 +6298,7 @@
         <v>152</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -6322,7 +6322,7 @@
         <v>154</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -6346,7 +6346,7 @@
         <v>156</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -6370,7 +6370,7 @@
         <v>158</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -6394,7 +6394,7 @@
         <v>160</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -6442,7 +6442,7 @@
         <v>165</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -6457,7 +6457,7 @@
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>166</v>
@@ -6479,7 +6479,7 @@
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>167</v>
@@ -6526,7 +6526,7 @@
         <v>170</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -6554,7 +6554,7 @@
         <v>175</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>176</v>
@@ -6582,7 +6582,7 @@
         <v>175</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>179</v>
@@ -6601,7 +6601,7 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>180</v>
@@ -6669,7 +6669,7 @@
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>185</v>
@@ -6715,7 +6715,7 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>187</v>
@@ -6739,7 +6739,7 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>189</v>
@@ -6763,7 +6763,7 @@
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>191</v>
@@ -6883,7 +6883,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
-      <formula>and($A45="end repeat", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
+      <formula>AND($A45="end repeat", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
@@ -7805,10 +7805,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.1581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="24.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28478,9 +28478,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.8877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.2397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="24.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28515,7 +28515,7 @@
       </c>
       <c r="C2" s="32" t="n">
         <f aca="true">NOW()</f>
-        <v>44098.7187694888</v>
+        <v>44098.740645434</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>833</v>

</xml_diff>